<commit_message>
Inner Product Experiments + AMS Synthetic Experiments
</commit_message>
<xml_diff>
--- a/Experiments/Experiments Status.xlsx
+++ b/Experiments/Experiments Status.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuval\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuval\Desktop\Distributed Monitoring Thesis\Experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4012F237-A233-4494-B691-BA640F4444A1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF1E2E2-EDCC-4F27-90AE-F096459F0B86}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>Function</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Pending Dani's Decision</t>
+  </si>
+  <si>
+    <t>Bandwidth of general function monitoring doesn't reflect the distance vs value difference, though another measurement of the time of the first full sync produces good result</t>
   </si>
 </sst>
 </file>
@@ -108,7 +111,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,8 +160,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDEC8EE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -181,34 +196,282 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -219,6 +482,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFDEC8EE"/>
       <color rgb="FF97E4FF"/>
       <color rgb="FFFF7575"/>
     </mruColors>
@@ -497,114 +761,116 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:E7"/>
+  <dimension ref="B1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="5" width="30.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="6" width="30.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="2:6" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="2:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="B3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="18" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="6"/>
+      <c r="F4" s="19"/>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="2:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="B5" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="6"/>
+      <c r="F5" s="19"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="C6" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="D6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="E6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="6"/>
+      <c r="F6" s="19"/>
     </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="2:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="6"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E3:E7"/>
+    <mergeCell ref="F3:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>